<commit_message>
NC92Soil - Versione 0.6
- Implementata analisi batch senza permutazioni (con input a Vs fissa o variabile con la profondità)
</commit_message>
<xml_diff>
--- a/Batch analysis.xlsx
+++ b/Batch analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97A79E9-3EEE-4AF0-97FD-16CAF4111275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403FB160-79A9-473B-8A7A-6D93307B4B78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Soils" sheetId="1" r:id="rId1"/>
     <sheet name="Clusters" sheetId="4" r:id="rId2"/>
+    <sheet name="Profiles" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Soil name</t>
   </si>
@@ -107,6 +108,36 @@
   </si>
   <si>
     <t>SUB2</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>A;9;250</t>
+  </si>
+  <si>
+    <t>B;8;300</t>
+  </si>
+  <si>
+    <t>A;3;350</t>
+  </si>
+  <si>
+    <t>A;5</t>
+  </si>
+  <si>
+    <t>B;9</t>
+  </si>
+  <si>
+    <t>A;8</t>
+  </si>
+  <si>
+    <t>B;3</t>
   </si>
 </sst>
 </file>
@@ -484,7 +515,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +727,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +802,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -784,6 +815,82 @@
       </c>
       <c r="H3" s="3">
         <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F31575F-4F45-4D8D-893C-5751BBD84B2E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NC92Soil - Versione 0.6 bis
- Implementata gestione ottimizzata delle permutazioni in modo da calcolarle una sola volta per ogni cluster
- Corretto bug che provocava la creazione di più export identici nel caso di DH se il foglio Soils conteneva più percentili per la Vs
</commit_message>
<xml_diff>
--- a/Batch analysis.xlsx
+++ b/Batch analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403FB160-79A9-473B-8A7A-6D93307B4B78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25A5284-25CD-4BB0-AA24-F90AC8A0E826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Soils" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Soil name</t>
   </si>
@@ -110,34 +104,58 @@
     <t>SUB2</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
     <t>A;9;250</t>
   </si>
   <si>
-    <t>B;8;300</t>
-  </si>
-  <si>
     <t>A;3;350</t>
   </si>
   <si>
     <t>A;5</t>
   </si>
   <si>
-    <t>B;9</t>
-  </si>
-  <si>
-    <t>A;8</t>
-  </si>
-  <si>
-    <t>B;3</t>
+    <t>G;3</t>
+  </si>
+  <si>
+    <t>G;8;300</t>
+  </si>
+  <si>
+    <t>G;9</t>
+  </si>
+  <si>
+    <t>SUB3</t>
+  </si>
+  <si>
+    <t>DH1</t>
+  </si>
+  <si>
+    <t>A;5;250</t>
+  </si>
+  <si>
+    <t>G;9;320</t>
+  </si>
+  <si>
+    <t>A;8;380</t>
+  </si>
+  <si>
+    <t>SOND1</t>
+  </si>
+  <si>
+    <t>SOND2</t>
+  </si>
+  <si>
+    <t>Spettro UHS 3.txt</t>
+  </si>
+  <si>
+    <t>S;5</t>
+  </si>
+  <si>
+    <t>A;7</t>
+  </si>
+  <si>
+    <t>G;10</t>
+  </si>
+  <si>
+    <t>DH2</t>
   </si>
 </sst>
 </file>
@@ -189,14 +207,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077C68C1-2C36-4D1D-BFFD-EAE68761E3D7}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,82 +757,108 @@
     <col min="5" max="5" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>30</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>30</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>30</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="5">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3">
+      <c r="C3" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5">
         <v>60</v>
       </c>
-      <c r="G3" s="3">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3">
-        <v>20</v>
+      <c r="G3" s="5">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5">
+        <v>33</v>
+      </c>
+      <c r="H4" s="5">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -825,31 +869,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F31575F-4F45-4D8D-893C-5751BBD84B2E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -859,38 +906,50 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="D5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NC92Soil Versione 0.7 del 22/09/2020
- Implementato generatore di profili stocastici su file Excel per input batch con media di Vs variabile con la profondità e correlazione tra i layer
- Implementato parser per espressioni arbitrarie per la media delle Vs e per la correlazione
- Implementata possibilità di applicare la correlazione all'intero profilo o ai singoli gruppi indipendentemente
</commit_message>
<xml_diff>
--- a/Batch analysis.xlsx
+++ b/Batch analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25A5284-25CD-4BB0-AA24-F90AC8A0E826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFAD064-DF9E-472C-AD3D-136F249E82BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Soils" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Soil name</t>
   </si>
@@ -95,67 +95,7 @@
     <t>350; 450; 550; 650</t>
   </si>
   <si>
-    <t>Spettro UHS 2.txt; Spettro UHS 3.txt</t>
-  </si>
-  <si>
     <t>Spettro UHS 2.txt</t>
-  </si>
-  <si>
-    <t>SUB2</t>
-  </si>
-  <si>
-    <t>A;9;250</t>
-  </si>
-  <si>
-    <t>A;3;350</t>
-  </si>
-  <si>
-    <t>A;5</t>
-  </si>
-  <si>
-    <t>G;3</t>
-  </si>
-  <si>
-    <t>G;8;300</t>
-  </si>
-  <si>
-    <t>G;9</t>
-  </si>
-  <si>
-    <t>SUB3</t>
-  </si>
-  <si>
-    <t>DH1</t>
-  </si>
-  <si>
-    <t>A;5;250</t>
-  </si>
-  <si>
-    <t>G;9;320</t>
-  </si>
-  <si>
-    <t>A;8;380</t>
-  </si>
-  <si>
-    <t>SOND1</t>
-  </si>
-  <si>
-    <t>SOND2</t>
-  </si>
-  <si>
-    <t>Spettro UHS 3.txt</t>
-  </si>
-  <si>
-    <t>S;5</t>
-  </si>
-  <si>
-    <t>A;7</t>
-  </si>
-  <si>
-    <t>G;10</t>
-  </si>
-  <si>
-    <t>DH2</t>
   </si>
 </sst>
 </file>
@@ -533,7 +473,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,10 +682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077C68C1-2C36-4D1D-BFFD-EAE68761E3D7}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,71 +734,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5">
-        <v>30</v>
+        <v>33.33</v>
       </c>
       <c r="G2" s="5">
-        <v>30</v>
+        <v>33.33</v>
       </c>
       <c r="H2" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5">
-        <v>60</v>
-      </c>
-      <c r="G3" s="5">
-        <v>20</v>
-      </c>
-      <c r="H3" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="5">
-        <v>33</v>
-      </c>
-      <c r="G4" s="5">
-        <v>33</v>
-      </c>
-      <c r="H4" s="5">
-        <v>33</v>
+        <v>33.33</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +757,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F31575F-4F45-4D8D-893C-5751BBD84B2E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,78 +769,7 @@
     <col min="2" max="3" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>